<commit_message>
atualizei nma com os codigos corretos. no final do script add um plot para poder fazer avaliacao da confiabilidade das comparacoes da nma de rato manualmente.
</commit_message>
<xml_diff>
--- a/data/nma_contrib_c.xlsx
+++ b/data/nma_contrib_c.xlsx
@@ -401,19 +401,19 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.1511848283917633</v>
+        <v>0.1513143487710279</v>
       </c>
       <c r="C2">
-        <v>0.2732227574123547</v>
+        <v>0.2730284768434579</v>
       </c>
       <c r="D2">
-        <v>0.4244075858041181</v>
+        <v>0.4243428256144858</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.1511848283917633</v>
+        <v>0.1513143487710279</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -426,19 +426,19 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.1511848283917633</v>
+        <v>0.151314348771028</v>
       </c>
       <c r="C3">
-        <v>0.2732227574123548</v>
+        <v>0.2730284768434579</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.4244075858041181</v>
+        <v>0.4243428256144859</v>
       </c>
       <c r="F3">
-        <v>0.1511848283917633</v>
+        <v>0.151314348771028</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -451,10 +451,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.5480894520895122</v>
+        <v>0.5477608887565193</v>
       </c>
       <c r="C4">
-        <v>0.2259552739552439</v>
+        <v>0.2261195556217403</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -463,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.2259552739552439</v>
+        <v>0.2261195556217403</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.1511848283917633</v>
+        <v>0.151314348771028</v>
       </c>
       <c r="C5">
-        <v>0.2732227574123548</v>
+        <v>0.2730284768434579</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -488,10 +488,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.1511848283917633</v>
+        <v>0.151314348771028</v>
       </c>
       <c r="G5">
-        <v>0.4244075858041181</v>
+        <v>0.424342825614486</v>
       </c>
     </row>
     <row r="6">
@@ -501,10 +501,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.226777242587645</v>
+        <v>0.2269715231565421</v>
       </c>
       <c r="C6">
-        <v>0.5464455148247096</v>
+        <v>0.546056953686916</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.226777242587645</v>
+        <v>0.2269715231565421</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -551,19 +551,19 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.03151165563807391</v>
+        <v>0.03127261414781171</v>
       </c>
       <c r="C8">
-        <v>0.03151165563807391</v>
+        <v>0.03127261414781171</v>
       </c>
       <c r="D8">
-        <v>0.4842441721809631</v>
+        <v>0.4843636929260938</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.4527325165428892</v>
+        <v>0.4530910787782821</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.4999999999999999</v>
+        <v>0.4999999999999998</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -591,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.4999999999999999</v>
+        <v>0.4999999999999998</v>
       </c>
     </row>
     <row r="10">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.03151165563807395</v>
+        <v>0.03127261414781165</v>
       </c>
       <c r="C11">
-        <v>0.03151165563807395</v>
+        <v>0.03127261414781165</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.4842441721809631</v>
+        <v>0.4843636929260943</v>
       </c>
       <c r="F11">
-        <v>0.4527325165428892</v>
+        <v>0.4530910787782826</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.03151165563807393</v>
+        <v>0.03127261414781168</v>
       </c>
       <c r="C14">
-        <v>0.03151165563807393</v>
+        <v>0.03127261414781168</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -713,10 +713,10 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.452732516542889</v>
+        <v>0.4530910787782825</v>
       </c>
       <c r="G14">
-        <v>0.4842441721809629</v>
+        <v>0.4843636929260942</v>
       </c>
     </row>
     <row r="15">
@@ -726,10 +726,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.04726748345711092</v>
+        <v>0.04690892122171759</v>
       </c>
       <c r="C15">
-        <v>0.04726748345711092</v>
+        <v>0.04690892122171759</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.9054650330857782</v>
+        <v>0.9061821575565647</v>
       </c>
       <c r="G15">
         <v>0</v>

</xml_diff>